<commit_message>
file dialog and json conversion implemented
</commit_message>
<xml_diff>
--- a/160603_ExcelLibraryEditor.xlsx
+++ b/160603_ExcelLibraryEditor.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="5930" tabRatio="737" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="5930" tabRatio="737"/>
   </bookViews>
   <sheets>
     <sheet name="OpaqueMaterial" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="253">
   <si>
     <t>[lambda  rho c: U-Wert.net] [LCA ICE,  General Clay data]</t>
   </si>
@@ -837,6 +837,45 @@
   </si>
   <si>
     <t>Partition</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [lambda  rho c: dataholz.com] [ LCA ICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GypsumFibreBoard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Boards</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cross Laminated Timber</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Timber</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mineral Wool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bonded chippings</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Impact sound insulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [lambda  rho c: Saint-Gobain Rigips][LCA  ICE (0.31fos + 0.41bio-embodied cabon emissions)]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [lambda  rho c: dataholz.com][LCA  ICE (0.31fos + 0.41bio-embodied cabon emissions)]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [lambda  rho c: dataholz.com]</t>
   </si>
 </sst>
 </file>
@@ -1216,10 +1255,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W87" sqref="W87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3581,6 +3621,323 @@
       </c>
       <c r="L62" s="2" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>241</v>
+      </c>
+      <c r="B64" t="s">
+        <v>242</v>
+      </c>
+      <c r="C64">
+        <v>0.32</v>
+      </c>
+      <c r="D64">
+        <v>1000</v>
+      </c>
+      <c r="E64">
+        <v>1100</v>
+      </c>
+      <c r="F64">
+        <v>0.9</v>
+      </c>
+      <c r="G64">
+        <v>0.7</v>
+      </c>
+      <c r="H64">
+        <v>0.7</v>
+      </c>
+      <c r="I64">
+        <v>45</v>
+      </c>
+      <c r="J64">
+        <v>1.86</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>243</v>
+      </c>
+      <c r="B65" t="s">
+        <v>244</v>
+      </c>
+      <c r="C65">
+        <v>0.13</v>
+      </c>
+      <c r="D65">
+        <v>500</v>
+      </c>
+      <c r="E65">
+        <v>1600</v>
+      </c>
+      <c r="F65">
+        <v>0.9</v>
+      </c>
+      <c r="G65">
+        <v>0.7</v>
+      </c>
+      <c r="H65">
+        <v>0.7</v>
+      </c>
+      <c r="I65">
+        <v>10</v>
+      </c>
+      <c r="J65">
+        <v>0.71</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" t="s">
+        <v>58</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>2000</v>
+      </c>
+      <c r="E66">
+        <v>1130</v>
+      </c>
+      <c r="F66">
+        <v>0.9</v>
+      </c>
+      <c r="G66">
+        <v>0.6</v>
+      </c>
+      <c r="H66">
+        <v>0.6</v>
+      </c>
+      <c r="I66">
+        <v>1.33</v>
+      </c>
+      <c r="J66">
+        <v>0.221</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>245</v>
+      </c>
+      <c r="B67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="D67">
+        <v>155</v>
+      </c>
+      <c r="E67">
+        <v>1130</v>
+      </c>
+      <c r="F67">
+        <v>0.9</v>
+      </c>
+      <c r="G67">
+        <v>0.6</v>
+      </c>
+      <c r="H67">
+        <v>0.6</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D68">
+        <v>35</v>
+      </c>
+      <c r="E68">
+        <v>1400</v>
+      </c>
+      <c r="F68">
+        <v>0.9</v>
+      </c>
+      <c r="G68">
+        <v>0.6</v>
+      </c>
+      <c r="H68">
+        <v>0.6</v>
+      </c>
+      <c r="I68">
+        <v>87.4</v>
+      </c>
+      <c r="J68">
+        <v>2.8</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D69">
+        <v>1200</v>
+      </c>
+      <c r="E69">
+        <v>1000</v>
+      </c>
+      <c r="F69">
+        <v>0.9</v>
+      </c>
+      <c r="G69">
+        <v>0.6</v>
+      </c>
+      <c r="H69">
+        <v>0.6</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>246</v>
+      </c>
+      <c r="B70" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70">
+        <v>0.7</v>
+      </c>
+      <c r="D70">
+        <v>1800</v>
+      </c>
+      <c r="E70">
+        <v>1000</v>
+      </c>
+      <c r="F70">
+        <v>0.9</v>
+      </c>
+      <c r="G70">
+        <v>0.6</v>
+      </c>
+      <c r="H70">
+        <v>0.6</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>247</v>
+      </c>
+      <c r="B71" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D71">
+        <v>120</v>
+      </c>
+      <c r="E71">
+        <v>1030</v>
+      </c>
+      <c r="F71">
+        <v>0.9</v>
+      </c>
+      <c r="G71">
+        <v>0.6</v>
+      </c>
+      <c r="H71">
+        <v>0.6</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -5167,8 +5524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5263,8 +5620,9 @@
       <c r="E4" t="s">
         <v>36</v>
       </c>
-      <c r="F4" t="s">
-        <v>44</v>
+      <c r="F4" t="str">
+        <f>OpaqueMaterial!A35</f>
+        <v>Styrofoam</v>
       </c>
       <c r="G4" t="s">
         <v>45</v>

</xml_diff>